<commit_message>
Just output.txt and report... if it commits
</commit_message>
<xml_diff>
--- a/GEDCOM_JAVA/Team04Report.xlsx
+++ b/GEDCOM_JAVA/Team04Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="11020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="11025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="101">
   <si>
     <t>Initials</t>
   </si>
@@ -55,6 +55,7 @@
         <sz val="10"/>
         <color indexed="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t>hchaturv@stevens.edu</t>
     </r>
@@ -78,6 +79,7 @@
         <sz val="10"/>
         <color indexed="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t>sgrozny@stevens.edu</t>
     </r>
@@ -95,6 +97,7 @@
         <sz val="10"/>
         <color indexed="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t>lzhang40@stevens.edu</t>
     </r>
@@ -310,12 +313,6 @@
     <t>Keep doing:</t>
   </si>
   <si>
-    <t>Meet twice a week</t>
-  </si>
-  <si>
-    <t>Text everyone when you discover a problem</t>
-  </si>
-  <si>
     <t>Avoid:</t>
   </si>
   <si>
@@ -350,6 +347,12 @@
   </si>
   <si>
     <t>gender on parents</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Meeting only once a week</t>
   </si>
 </sst>
 </file>
@@ -370,28 +373,33 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -599,7 +607,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -779,7 +787,7 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24</c:v>
@@ -808,11 +816,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110441600"/>
-        <c:axId val="110443136"/>
+        <c:axId val="93226112"/>
+        <c:axId val="104173568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110441600"/>
+        <c:axId val="93226112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110443136"/>
+        <c:crossAx val="104173568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -855,7 +863,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110443136"/>
+        <c:axId val="104173568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,7 +909,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110441600"/>
+        <c:crossAx val="93226112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7.5"/>
@@ -2226,16 +2234,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
     <col min="2" max="3" width="7.59765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="6" width="24.1328125" style="1" customWidth="1"/>
-    <col min="7" max="256" width="8.1328125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="24.09765625" style="1" customWidth="1"/>
+    <col min="7" max="256" width="8.09765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2253,7 +2261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2261,7 +2269,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="6" t="s">
         <v>5</v>
@@ -2279,7 +2287,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="6" t="s">
         <v>10</v>
@@ -2297,16 +2305,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>16</v>
@@ -2315,7 +2323,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2323,7 +2331,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2331,7 +2339,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2339,7 +2347,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2351,7 +2359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2379,12 +2387,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="8.1328125" style="31" customWidth="1"/>
+    <col min="1" max="256" width="8.09765625" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -2416,7 +2424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2428,7 +2436,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2440,7 +2448,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2452,7 +2460,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2464,7 +2472,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2476,7 +2484,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2488,7 +2496,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2500,7 +2508,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2512,7 +2520,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2538,27 +2546,27 @@
   <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G2" sqref="G2:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.86328125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="5.73046875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="3.8984375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="5.69921875" style="8" customWidth="1"/>
     <col min="3" max="3" width="14.59765625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="7.265625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="7.296875" style="8" customWidth="1"/>
     <col min="5" max="5" width="5" style="8" customWidth="1"/>
-    <col min="6" max="6" width="5.73046875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="5.1328125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="5.69921875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.09765625" style="8" customWidth="1"/>
     <col min="8" max="8" width="5.59765625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="5.46484375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="5.86328125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="5.5" style="8" customWidth="1"/>
+    <col min="10" max="10" width="5.8984375" style="8" customWidth="1"/>
     <col min="11" max="11" width="7.3984375" style="8" customWidth="1"/>
     <col min="12" max="12" width="8" style="8" customWidth="1"/>
-    <col min="13" max="256" width="8.1328125" style="8" customWidth="1"/>
+    <col min="13" max="256" width="8.09765625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -2596,7 +2604,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2604,11 +2612,11 @@
         <v>32</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>37</v>
@@ -2622,7 +2630,7 @@
       <c r="I2" s="5">
         <v>23</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="6">
         <v>30</v>
       </c>
       <c r="K2" s="10">
@@ -2630,7 +2638,7 @@
       </c>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2642,7 +2650,7 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>37</v>
@@ -2664,7 +2672,7 @@
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -2698,7 +2706,7 @@
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -2732,7 +2740,7 @@
       </c>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -2766,7 +2774,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
         <v>42</v>
@@ -2782,7 +2790,7 @@
       <c r="K7" s="10"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
         <v>43</v>
@@ -2798,7 +2806,7 @@
       <c r="K8" s="10"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>44</v>
@@ -2814,7 +2822,7 @@
       <c r="K9" s="10"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
         <v>45</v>
@@ -2844,21 +2852,21 @@
   <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="6.09765625" style="12" customWidth="1"/>
     <col min="2" max="2" width="17" style="12" customWidth="1"/>
-    <col min="3" max="3" width="48.265625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="8.1328125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="6.1328125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="48.296875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="8.09765625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="6.09765625" style="12" customWidth="1"/>
     <col min="6" max="6" width="6.3984375" style="12" customWidth="1"/>
-    <col min="7" max="256" width="8.1328125" style="12" customWidth="1"/>
+    <col min="7" max="256" width="8.09765625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -2878,18 +2886,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="26.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E2" s="5">
         <v>15</v>
@@ -2898,7 +2906,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -2909,7 +2917,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E3" s="5">
         <v>20</v>
@@ -2918,7 +2926,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="26.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
@@ -2932,13 +2940,13 @@
         <v>50</v>
       </c>
       <c r="E4" s="5">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F4" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -2958,7 +2966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
@@ -2972,13 +2980,13 @@
         <v>55</v>
       </c>
       <c r="E6" s="5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F6" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -2988,7 +2996,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -2998,7 +3006,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="15"/>
@@ -3006,7 +3014,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="15"/>
@@ -3028,21 +3036,21 @@
   <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.59765625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="5.86328125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="5.8984375" style="16" customWidth="1"/>
     <col min="3" max="3" width="14" style="16" customWidth="1"/>
-    <col min="4" max="4" width="24.1328125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="24.09765625" style="16" customWidth="1"/>
     <col min="5" max="5" width="24.3984375" style="16" customWidth="1"/>
     <col min="6" max="6" width="16.3984375" style="16" customWidth="1"/>
-    <col min="7" max="256" width="8.1328125" style="16" customWidth="1"/>
+    <col min="7" max="256" width="8.09765625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -3062,7 +3070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>59</v>
       </c>
@@ -3070,19 +3078,19 @@
         <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
@@ -3093,16 +3101,16 @@
         <v>34</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>61</v>
       </c>
@@ -3122,7 +3130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>65</v>
       </c>
@@ -3142,7 +3150,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>70</v>
       </c>
@@ -3162,7 +3170,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>74</v>
       </c>
@@ -3174,7 +3182,7 @@
       <c r="E7" s="18"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>75</v>
       </c>
@@ -3186,7 +3194,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>76</v>
       </c>
@@ -3198,7 +3206,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>77</v>
       </c>
@@ -3223,20 +3231,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" style="24" customWidth="1"/>
-    <col min="2" max="2" width="12.46484375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="24" customWidth="1"/>
     <col min="3" max="3" width="9.3984375" style="24" customWidth="1"/>
     <col min="4" max="4" width="5.3984375" style="24" customWidth="1"/>
-    <col min="5" max="5" width="8.9296875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" style="24" customWidth="1"/>
     <col min="6" max="6" width="9.3984375" style="24" customWidth="1"/>
-    <col min="7" max="256" width="8.1328125" style="24" customWidth="1"/>
+    <col min="7" max="256" width="8.09765625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
@@ -3256,7 +3266,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>40590</v>
       </c>
@@ -3270,29 +3280,31 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>40604</v>
       </c>
       <c r="B3" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6">
         <f>B2-B3</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="6">
-        <v>53</v>
+        <f>SUM(Sprint1!H2:H6)</f>
+        <v>119</v>
       </c>
       <c r="E3" s="6">
-        <v>40</v>
+        <f>SUM(Sprint1!I2:I6)</f>
+        <v>171</v>
       </c>
       <c r="F3" s="25">
         <f>(D3-D2)/E3*60</f>
-        <v>79.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>41.754385964912281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>40625</v>
       </c>
@@ -3301,7 +3313,7 @@
       </c>
       <c r="C4" s="6">
         <f>B3-B4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
@@ -3314,7 +3326,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>40639</v>
       </c>
@@ -3336,7 +3348,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>40653</v>
       </c>
@@ -3358,7 +3370,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>40667</v>
       </c>
@@ -3380,7 +3392,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3388,7 +3400,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -3396,7 +3408,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -3416,28 +3428,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV21"/>
+  <dimension ref="A1:IV22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I2" sqref="I2:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.73046875" style="26" customWidth="1"/>
+    <col min="1" max="1" width="5.69921875" style="26" customWidth="1"/>
     <col min="2" max="2" width="18.3984375" style="26" customWidth="1"/>
-    <col min="3" max="3" width="8.73046875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" style="26" customWidth="1"/>
     <col min="4" max="4" width="5" style="26" customWidth="1"/>
-    <col min="5" max="5" width="8.1328125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="5.1328125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="8.09765625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="5.09765625" style="26" customWidth="1"/>
     <col min="7" max="7" width="5.59765625" style="26" customWidth="1"/>
     <col min="8" max="8" width="5" style="26" customWidth="1"/>
-    <col min="9" max="9" width="5.73046875" style="26" customWidth="1"/>
+    <col min="9" max="9" width="5.69921875" style="26" customWidth="1"/>
     <col min="10" max="10" width="8" style="26" customWidth="1"/>
-    <col min="11" max="256" width="8.1328125" style="26" customWidth="1"/>
+    <col min="11" max="256" width="8.09765625" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -3469,18 +3481,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>37</v>
@@ -3491,7 +3503,7 @@
       <c r="G2" s="6">
         <v>49</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>23</v>
       </c>
       <c r="I2" s="6">
@@ -3501,7 +3513,7 @@
         <v>40604</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -3509,13 +3521,13 @@
         <v>34</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="F3" s="5">
         <v>20</v>
@@ -3529,25 +3541,287 @@
       <c r="I3" s="5">
         <v>61</v>
       </c>
-      <c r="J3" s="5">
-        <v>40604</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="5">
+        <v>25</v>
+      </c>
+      <c r="G4" s="5">
+        <v>30</v>
+      </c>
+      <c r="H4" s="5">
+        <v>25</v>
+      </c>
+      <c r="I4" s="5">
+        <v>30</v>
+      </c>
+      <c r="J4" s="10">
+        <v>40604</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="31"/>
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="31"/>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="31"/>
+      <c r="AJ4" s="31"/>
+      <c r="AK4" s="31"/>
+      <c r="AL4" s="31"/>
+      <c r="AM4" s="31"/>
+      <c r="AN4" s="31"/>
+      <c r="AO4" s="31"/>
+      <c r="AP4" s="31"/>
+      <c r="AQ4" s="31"/>
+      <c r="AR4" s="31"/>
+      <c r="AS4" s="31"/>
+      <c r="AT4" s="31"/>
+      <c r="AU4" s="31"/>
+      <c r="AV4" s="31"/>
+      <c r="AW4" s="31"/>
+      <c r="AX4" s="31"/>
+      <c r="AY4" s="31"/>
+      <c r="AZ4" s="31"/>
+      <c r="BA4" s="31"/>
+      <c r="BB4" s="31"/>
+      <c r="BC4" s="31"/>
+      <c r="BD4" s="31"/>
+      <c r="BE4" s="31"/>
+      <c r="BF4" s="31"/>
+      <c r="BG4" s="31"/>
+      <c r="BH4" s="31"/>
+      <c r="BI4" s="31"/>
+      <c r="BJ4" s="31"/>
+      <c r="BK4" s="31"/>
+      <c r="BL4" s="31"/>
+      <c r="BM4" s="31"/>
+      <c r="BN4" s="31"/>
+      <c r="BO4" s="31"/>
+      <c r="BP4" s="31"/>
+      <c r="BQ4" s="31"/>
+      <c r="BR4" s="31"/>
+      <c r="BS4" s="31"/>
+      <c r="BT4" s="31"/>
+      <c r="BU4" s="31"/>
+      <c r="BV4" s="31"/>
+      <c r="BW4" s="31"/>
+      <c r="BX4" s="31"/>
+      <c r="BY4" s="31"/>
+      <c r="BZ4" s="31"/>
+      <c r="CA4" s="31"/>
+      <c r="CB4" s="31"/>
+      <c r="CC4" s="31"/>
+      <c r="CD4" s="31"/>
+      <c r="CE4" s="31"/>
+      <c r="CF4" s="31"/>
+      <c r="CG4" s="31"/>
+      <c r="CH4" s="31"/>
+      <c r="CI4" s="31"/>
+      <c r="CJ4" s="31"/>
+      <c r="CK4" s="31"/>
+      <c r="CL4" s="31"/>
+      <c r="CM4" s="31"/>
+      <c r="CN4" s="31"/>
+      <c r="CO4" s="31"/>
+      <c r="CP4" s="31"/>
+      <c r="CQ4" s="31"/>
+      <c r="CR4" s="31"/>
+      <c r="CS4" s="31"/>
+      <c r="CT4" s="31"/>
+      <c r="CU4" s="31"/>
+      <c r="CV4" s="31"/>
+      <c r="CW4" s="31"/>
+      <c r="CX4" s="31"/>
+      <c r="CY4" s="31"/>
+      <c r="CZ4" s="31"/>
+      <c r="DA4" s="31"/>
+      <c r="DB4" s="31"/>
+      <c r="DC4" s="31"/>
+      <c r="DD4" s="31"/>
+      <c r="DE4" s="31"/>
+      <c r="DF4" s="31"/>
+      <c r="DG4" s="31"/>
+      <c r="DH4" s="31"/>
+      <c r="DI4" s="31"/>
+      <c r="DJ4" s="31"/>
+      <c r="DK4" s="31"/>
+      <c r="DL4" s="31"/>
+      <c r="DM4" s="31"/>
+      <c r="DN4" s="31"/>
+      <c r="DO4" s="31"/>
+      <c r="DP4" s="31"/>
+      <c r="DQ4" s="31"/>
+      <c r="DR4" s="31"/>
+      <c r="DS4" s="31"/>
+      <c r="DT4" s="31"/>
+      <c r="DU4" s="31"/>
+      <c r="DV4" s="31"/>
+      <c r="DW4" s="31"/>
+      <c r="DX4" s="31"/>
+      <c r="DY4" s="31"/>
+      <c r="DZ4" s="31"/>
+      <c r="EA4" s="31"/>
+      <c r="EB4" s="31"/>
+      <c r="EC4" s="31"/>
+      <c r="ED4" s="31"/>
+      <c r="EE4" s="31"/>
+      <c r="EF4" s="31"/>
+      <c r="EG4" s="31"/>
+      <c r="EH4" s="31"/>
+      <c r="EI4" s="31"/>
+      <c r="EJ4" s="31"/>
+      <c r="EK4" s="31"/>
+      <c r="EL4" s="31"/>
+      <c r="EM4" s="31"/>
+      <c r="EN4" s="31"/>
+      <c r="EO4" s="31"/>
+      <c r="EP4" s="31"/>
+      <c r="EQ4" s="31"/>
+      <c r="ER4" s="31"/>
+      <c r="ES4" s="31"/>
+      <c r="ET4" s="31"/>
+      <c r="EU4" s="31"/>
+      <c r="EV4" s="31"/>
+      <c r="EW4" s="31"/>
+      <c r="EX4" s="31"/>
+      <c r="EY4" s="31"/>
+      <c r="EZ4" s="31"/>
+      <c r="FA4" s="31"/>
+      <c r="FB4" s="31"/>
+      <c r="FC4" s="31"/>
+      <c r="FD4" s="31"/>
+      <c r="FE4" s="31"/>
+      <c r="FF4" s="31"/>
+      <c r="FG4" s="31"/>
+      <c r="FH4" s="31"/>
+      <c r="FI4" s="31"/>
+      <c r="FJ4" s="31"/>
+      <c r="FK4" s="31"/>
+      <c r="FL4" s="31"/>
+      <c r="FM4" s="31"/>
+      <c r="FN4" s="31"/>
+      <c r="FO4" s="31"/>
+      <c r="FP4" s="31"/>
+      <c r="FQ4" s="31"/>
+      <c r="FR4" s="31"/>
+      <c r="FS4" s="31"/>
+      <c r="FT4" s="31"/>
+      <c r="FU4" s="31"/>
+      <c r="FV4" s="31"/>
+      <c r="FW4" s="31"/>
+      <c r="FX4" s="31"/>
+      <c r="FY4" s="31"/>
+      <c r="FZ4" s="31"/>
+      <c r="GA4" s="31"/>
+      <c r="GB4" s="31"/>
+      <c r="GC4" s="31"/>
+      <c r="GD4" s="31"/>
+      <c r="GE4" s="31"/>
+      <c r="GF4" s="31"/>
+      <c r="GG4" s="31"/>
+      <c r="GH4" s="31"/>
+      <c r="GI4" s="31"/>
+      <c r="GJ4" s="31"/>
+      <c r="GK4" s="31"/>
+      <c r="GL4" s="31"/>
+      <c r="GM4" s="31"/>
+      <c r="GN4" s="31"/>
+      <c r="GO4" s="31"/>
+      <c r="GP4" s="31"/>
+      <c r="GQ4" s="31"/>
+      <c r="GR4" s="31"/>
+      <c r="GS4" s="31"/>
+      <c r="GT4" s="31"/>
+      <c r="GU4" s="31"/>
+      <c r="GV4" s="31"/>
+      <c r="GW4" s="31"/>
+      <c r="GX4" s="31"/>
+      <c r="GY4" s="31"/>
+      <c r="GZ4" s="31"/>
+      <c r="HA4" s="31"/>
+      <c r="HB4" s="31"/>
+      <c r="HC4" s="31"/>
+      <c r="HD4" s="31"/>
+      <c r="HE4" s="31"/>
+      <c r="HF4" s="31"/>
+      <c r="HG4" s="31"/>
+      <c r="HH4" s="31"/>
+      <c r="HI4" s="31"/>
+      <c r="HJ4" s="31"/>
+      <c r="HK4" s="31"/>
+      <c r="HL4" s="31"/>
+      <c r="HM4" s="31"/>
+      <c r="HN4" s="31"/>
+      <c r="HO4" s="31"/>
+      <c r="HP4" s="31"/>
+      <c r="HQ4" s="31"/>
+      <c r="HR4" s="31"/>
+      <c r="HS4" s="31"/>
+      <c r="HT4" s="31"/>
+      <c r="HU4" s="31"/>
+      <c r="HV4" s="31"/>
+      <c r="HW4" s="31"/>
+      <c r="HX4" s="31"/>
+      <c r="HY4" s="31"/>
+      <c r="HZ4" s="31"/>
+      <c r="IA4" s="31"/>
+      <c r="IB4" s="31"/>
+      <c r="IC4" s="31"/>
+      <c r="ID4" s="31"/>
+      <c r="IE4" s="31"/>
+      <c r="IF4" s="31"/>
+      <c r="IG4" s="31"/>
+      <c r="IH4" s="31"/>
+      <c r="II4" s="31"/>
+      <c r="IJ4" s="31"/>
+      <c r="IK4" s="31"/>
+      <c r="IL4" s="31"/>
+      <c r="IM4" s="31"/>
+      <c r="IN4" s="31"/>
+      <c r="IO4" s="31"/>
+      <c r="IP4" s="31"/>
+      <c r="IQ4" s="31"/>
+      <c r="IR4" s="31"/>
+      <c r="IS4" s="31"/>
+      <c r="IT4" s="31"/>
+      <c r="IU4" s="31"/>
+      <c r="IV4"/>
+    </row>
+    <row r="5" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -3575,11 +3849,11 @@
       <c r="I5" s="5">
         <v>30</v>
       </c>
-      <c r="J5" s="5">
-        <v>40604</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="11">
+        <v>40607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:256" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
@@ -3607,9 +3881,11 @@
       <c r="I6" s="5">
         <v>20</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="11">
+        <v>40608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -3621,7 +3897,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -3633,7 +3909,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -3645,7 +3921,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="26.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:256" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -3657,7 +3933,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
@@ -3669,7 +3945,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="26.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:256" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -3681,7 +3957,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -3693,7 +3969,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="13" t="s">
         <v>85</v>
@@ -3707,7 +3983,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="27"/>
       <c r="C15" s="15"/>
@@ -3719,7 +3995,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="13" t="s">
         <v>86</v>
@@ -3733,11 +4009,9 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
-      <c r="B17" s="14" t="s">
-        <v>87</v>
-      </c>
+      <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -3747,11 +4021,9 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" ht="26.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
-      <c r="B18" s="14" t="s">
-        <v>88</v>
-      </c>
+      <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -3761,9 +4033,11 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="15"/>
+      <c r="B19" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="C19" s="15"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -3773,10 +4047,10 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
-      <c r="B20" s="13" t="s">
-        <v>89</v>
+      <c r="B20" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="5"/>
@@ -3787,10 +4061,10 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" ht="26.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="14" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="5"/>
@@ -3800,6 +4074,9 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3816,12 +4093,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="8.1328125" style="28" customWidth="1"/>
+    <col min="1" max="256" width="8.09765625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -3853,7 +4130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3865,7 +4142,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3877,7 +4154,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3889,7 +4166,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -3901,7 +4178,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3913,7 +4190,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -3925,7 +4202,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3937,7 +4214,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -3949,7 +4226,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -3976,12 +4253,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="8.1328125" style="29" customWidth="1"/>
+    <col min="1" max="256" width="8.09765625" style="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -4013,7 +4290,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -4025,7 +4302,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -4037,7 +4314,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4049,7 +4326,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -4061,7 +4338,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4073,7 +4350,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -4085,7 +4362,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -4097,7 +4374,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -4109,7 +4386,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -4136,12 +4413,12 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.1328125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.09765625" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="8.1328125" style="30" customWidth="1"/>
+    <col min="1" max="256" width="8.09765625" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -4173,7 +4450,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -4185,7 +4462,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -4197,7 +4474,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4209,7 +4486,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -4221,7 +4498,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4233,7 +4510,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -4245,7 +4522,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -4257,7 +4534,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -4269,7 +4546,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>

</xml_diff>